<commit_message>
updating results sheet for bigram networks
</commit_message>
<xml_diff>
--- a/docs/BIGRAMA_GERAL.xlsx
+++ b/docs/BIGRAMA_GERAL.xlsx
@@ -672,6 +672,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -688,9 +691,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:AC99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,39 +1114,39 @@
       <c r="A1" s="1"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="M6" s="30" t="s">
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="M6" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
     </row>
     <row r="7" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1204,7 +1204,9 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="K8" s="9">
+        <v>0.83618680000000001</v>
+      </c>
       <c r="M8" s="2">
         <v>172</v>
       </c>
@@ -1239,7 +1241,9 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="K9" s="9">
+        <v>0.83734629999999999</v>
+      </c>
       <c r="M9" s="2">
         <v>155.69999999999999</v>
       </c>
@@ -1273,7 +1277,9 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="9">
+        <v>0.83665959999999995</v>
+      </c>
       <c r="M10" s="2">
         <v>139.4</v>
       </c>
@@ -1738,32 +1744,32 @@
       <c r="K27" s="9"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29" t="s">
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
     </row>
     <row r="30" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="27"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="28"/>
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
@@ -1978,32 +1984,32 @@
       <c r="K36" s="9"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="29" t="s">
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
     </row>
     <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="27"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="28"/>
       <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
@@ -2220,32 +2226,32 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="28" t="s">
+      <c r="D45" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="29" t="s">
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
     </row>
     <row r="46" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="28"/>
       <c r="D46" s="3" t="s">
         <v>5</v>
       </c>
@@ -2455,32 +2461,32 @@
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D53" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="29" t="s">
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="30"/>
+      <c r="K53" s="30"/>
     </row>
     <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="27"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="28"/>
       <c r="D54" s="3" t="s">
         <v>5</v>
       </c>
@@ -2690,32 +2696,32 @@
       <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B61" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="28" t="s">
+      <c r="D61" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="29" t="s">
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I61" s="29"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="30"/>
     </row>
     <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="25"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="27"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="28"/>
       <c r="D62" s="3" t="s">
         <v>5</v>
       </c>
@@ -2925,32 +2931,32 @@
       <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="B69" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="26" t="s">
+      <c r="C69" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D69" s="28" t="s">
+      <c r="D69" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="29" t="s">
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I69" s="29"/>
-      <c r="J69" s="29"/>
-      <c r="K69" s="29"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
     </row>
     <row r="70" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="25"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="27"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="28"/>
       <c r="D70" s="3" t="s">
         <v>5</v>
       </c>
@@ -3160,32 +3166,32 @@
       <c r="G76" s="8"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="24" t="s">
+      <c r="A77" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="24" t="s">
+      <c r="B77" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="26" t="s">
+      <c r="C77" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="28" t="s">
+      <c r="D77" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="29" t="s">
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I77" s="29"/>
-      <c r="J77" s="29"/>
-      <c r="K77" s="29"/>
+      <c r="I77" s="30"/>
+      <c r="J77" s="30"/>
+      <c r="K77" s="30"/>
     </row>
     <row r="78" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="25"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="27"/>
+      <c r="A78" s="26"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="28"/>
       <c r="D78" s="3" t="s">
         <v>5</v>
       </c>
@@ -3395,32 +3401,32 @@
       <c r="G84" s="8"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="24" t="s">
+      <c r="A85" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B85" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="26" t="s">
+      <c r="C85" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="28" t="s">
+      <c r="D85" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="28"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="28"/>
-      <c r="H85" s="29" t="s">
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="29"/>
+      <c r="I85" s="30"/>
+      <c r="J85" s="30"/>
+      <c r="K85" s="30"/>
     </row>
     <row r="86" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="25"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="27"/>
+      <c r="A86" s="26"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="28"/>
       <c r="D86" s="3" t="s">
         <v>5</v>
       </c>
@@ -3630,32 +3636,32 @@
       <c r="G92" s="8"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" s="24" t="s">
+      <c r="A93" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="24" t="s">
+      <c r="B93" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C93" s="26" t="s">
+      <c r="C93" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D93" s="28" t="s">
+      <c r="D93" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="29" t="s">
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I93" s="29"/>
-      <c r="J93" s="29"/>
-      <c r="K93" s="29"/>
+      <c r="I93" s="30"/>
+      <c r="J93" s="30"/>
+      <c r="K93" s="30"/>
     </row>
     <row r="94" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="25"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="27"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="28"/>
       <c r="D94" s="3" t="s">
         <v>5</v>
       </c>
@@ -3858,6 +3864,46 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:G93"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:G77"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="H61:K61"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="H37:K37"/>
     <mergeCell ref="M6:Q6"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="B29:B30"/>
@@ -3869,46 +3915,6 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="H61:K61"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:G77"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:G93"/>
-    <mergeCell ref="H93:K93"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updating files for a second round of experiments with bigram vectors 2 layer deep neural nets
</commit_message>
<xml_diff>
--- a/docs/BIGRAMA_GERAL.xlsx
+++ b/docs/BIGRAMA_GERAL.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="102">
   <si>
     <t>Experimento</t>
   </si>
@@ -324,6 +324,15 @@
   </si>
   <si>
     <t>AE_BIGRAMA_10L_OVER_05</t>
+  </si>
+  <si>
+    <t>ESCOLHIDAS</t>
+  </si>
+  <si>
+    <t>AE_BIGRAMA_2L_OVER_02</t>
+  </si>
+  <si>
+    <t>AE_BIGRAMA_2L_OVER_03</t>
   </si>
 </sst>
 </file>
@@ -478,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -513,6 +522,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,17 +554,8 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,10 +952,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B1B422-5711-4894-8EC8-3356671E451B}">
-  <dimension ref="A1:AC99"/>
+  <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="W7" zoomScale="91" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,46 +970,70 @@
     <col min="9" max="9" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" style="2" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="12" max="22" width="8.88671875" style="2"/>
+    <col min="23" max="23" width="30.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" style="2"/>
+    <col min="26" max="26" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.5546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="M5" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="P5" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="M6" s="26" t="s">
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="M6" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-    </row>
-    <row r="7" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1024,26 +1059,32 @@
         <v>8</v>
       </c>
       <c r="M7" s="2">
-        <v>96</v>
+        <v>9216</v>
       </c>
       <c r="N7" s="2">
-        <v>96</v>
+        <v>9216</v>
       </c>
       <c r="O7" s="2">
-        <v>96</v>
+        <v>9216</v>
       </c>
       <c r="P7" s="17">
-        <v>96</v>
+        <v>9216</v>
       </c>
       <c r="Q7" s="17">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+        <v>9216</v>
+      </c>
+      <c r="W7" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="X7" s="8">
+        <v>0.83618680000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="6"/>
@@ -1060,27 +1101,32 @@
         <v>0.83618680000000001</v>
       </c>
       <c r="M8" s="2">
-        <v>172</v>
+        <v>15667</v>
       </c>
       <c r="N8" s="2">
-        <v>134</v>
+        <v>13824</v>
       </c>
       <c r="O8" s="2">
-        <v>86</v>
+        <v>5530</v>
       </c>
       <c r="P8" s="17">
-        <v>76</v>
+        <v>10138</v>
       </c>
       <c r="Q8" s="17">
-        <v>28</v>
-      </c>
-      <c r="X8" s="17"/>
-    </row>
-    <row r="9" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+        <v>14746</v>
+      </c>
+      <c r="W8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="X8" s="22">
+        <v>0.83734629999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="6"/>
@@ -1093,30 +1139,36 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="8">
+      <c r="K9" s="32">
         <v>0.83734629999999999</v>
       </c>
       <c r="M9" s="2">
-        <v>155.69999999999999</v>
+        <v>14101</v>
       </c>
       <c r="N9" s="2">
-        <v>121.5</v>
+        <v>12443</v>
       </c>
       <c r="O9" s="2">
-        <v>78.3</v>
+        <v>4978</v>
       </c>
       <c r="P9" s="17">
-        <v>69.3</v>
+        <v>9125</v>
       </c>
       <c r="Q9" s="17">
-        <v>26.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+        <v>13272</v>
+      </c>
+      <c r="W9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="X9" s="32">
+        <v>0.83665959999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="6"/>
@@ -1129,66 +1181,78 @@
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="8">
+      <c r="K10" s="32">
         <v>0.83665959999999995</v>
       </c>
       <c r="M10" s="2">
-        <v>139.4</v>
+        <v>12535</v>
       </c>
       <c r="N10" s="2">
-        <v>109</v>
+        <v>11061</v>
       </c>
       <c r="O10" s="2">
-        <v>70.599999999999994</v>
+        <v>4426</v>
       </c>
       <c r="P10" s="17">
-        <v>62.6</v>
+        <v>8112</v>
       </c>
       <c r="Q10" s="17">
-        <v>24.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
+        <v>11798</v>
+      </c>
+      <c r="W10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="X10" s="22">
+        <v>0.83724600000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9">
         <v>0.7166131</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29">
-        <v>0.85362459999999996</v>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="32">
+        <v>0.83724600000000005</v>
       </c>
       <c r="M11" s="2">
-        <v>123.1</v>
+        <v>10970</v>
       </c>
       <c r="N11" s="2">
-        <v>96.5</v>
+        <v>9680</v>
       </c>
       <c r="O11" s="2">
-        <v>62.9</v>
+        <v>3874</v>
       </c>
       <c r="P11" s="17">
-        <v>55.9</v>
+        <v>7099</v>
       </c>
       <c r="Q11" s="17">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
+        <v>10324</v>
+      </c>
+      <c r="W11" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="X11" s="32">
+        <v>0.83555539999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="6"/>
@@ -1201,30 +1265,36 @@
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="8">
+      <c r="K12" s="32">
         <v>0.83555539999999995</v>
       </c>
       <c r="M12" s="2">
-        <v>106.8</v>
+        <v>9404</v>
       </c>
       <c r="N12" s="2">
-        <v>84</v>
+        <v>8298</v>
       </c>
       <c r="O12" s="2">
-        <v>55.2</v>
+        <v>3322</v>
       </c>
       <c r="P12" s="17">
-        <v>49.2</v>
+        <v>6086</v>
       </c>
       <c r="Q12" s="17">
-        <v>20.400000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+        <v>8851</v>
+      </c>
+      <c r="W12" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="X12" s="22">
+        <v>0.83795830000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="6"/>
@@ -1237,30 +1307,36 @@
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="8">
+      <c r="K13" s="32">
         <v>0.83795830000000004</v>
       </c>
       <c r="M13" s="2">
-        <v>90.5</v>
+        <v>7838</v>
       </c>
       <c r="N13" s="2">
-        <v>71.5</v>
+        <v>6917</v>
       </c>
       <c r="O13" s="2">
-        <v>47.5</v>
+        <v>2770</v>
       </c>
       <c r="P13" s="17">
-        <v>42.5</v>
+        <v>5074</v>
       </c>
       <c r="Q13" s="17">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+        <v>7378</v>
+      </c>
+      <c r="W13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="X13" s="32">
+        <v>0.83634220000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="6"/>
@@ -1273,30 +1349,39 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="8">
+      <c r="K14" s="32">
         <v>0.83634220000000004</v>
       </c>
       <c r="M14" s="2">
-        <v>74.199999999999989</v>
+        <v>6272</v>
       </c>
       <c r="N14" s="2">
-        <v>59</v>
+        <v>5535</v>
       </c>
       <c r="O14" s="2">
-        <v>39.799999999999997</v>
+        <v>2217</v>
       </c>
       <c r="P14" s="17">
-        <v>35.799999999999997</v>
+        <v>4061</v>
       </c>
       <c r="Q14" s="17">
-        <v>16.600000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+        <v>5904</v>
+      </c>
+      <c r="W14" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="X14" s="32">
+        <v>0.83528259999999999</v>
+      </c>
+      <c r="AD14" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="6"/>
@@ -1309,30 +1394,39 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="8">
+      <c r="K15" s="32">
         <v>0.83528259999999999</v>
       </c>
       <c r="M15" s="2">
-        <v>57.899999999999991</v>
+        <v>4706</v>
       </c>
       <c r="N15" s="2">
-        <v>46.5</v>
+        <v>4154</v>
       </c>
       <c r="O15" s="2">
-        <v>32.1</v>
+        <v>1665</v>
       </c>
       <c r="P15" s="17">
-        <v>29.1</v>
+        <v>3048</v>
       </c>
       <c r="Q15" s="17">
-        <v>14.700000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+        <v>4430</v>
+      </c>
+      <c r="W15" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="X15" s="32">
+        <v>0.83638900000000005</v>
+      </c>
+      <c r="AD15" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="6"/>
@@ -1345,30 +1439,39 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="8">
+      <c r="K16" s="32">
         <v>0.83638900000000005</v>
       </c>
       <c r="M16" s="2">
-        <v>41.599999999999994</v>
+        <v>3141</v>
       </c>
       <c r="N16" s="2">
-        <v>34</v>
+        <v>2772</v>
       </c>
       <c r="O16" s="2">
-        <v>24.4</v>
+        <v>1113</v>
       </c>
       <c r="P16" s="17">
-        <v>22.4</v>
+        <v>2035</v>
       </c>
       <c r="Q16" s="17">
-        <v>12.800000000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+        <v>2956</v>
+      </c>
+      <c r="W16" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="X16" s="32">
+        <v>0.83698320000000004</v>
+      </c>
+      <c r="AD16" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="6"/>
@@ -1381,30 +1484,39 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="8">
+      <c r="K17" s="32">
         <v>0.83698320000000004</v>
       </c>
       <c r="M17" s="2">
-        <v>25.299999999999983</v>
+        <v>1575</v>
       </c>
       <c r="N17" s="2">
-        <v>21.5</v>
+        <v>1391</v>
       </c>
       <c r="O17" s="2">
-        <v>16.700000000000003</v>
+        <v>561</v>
       </c>
       <c r="P17" s="17">
-        <v>15.699999999999996</v>
+        <v>1022</v>
       </c>
       <c r="Q17" s="17">
-        <v>10.900000000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
+        <v>1483</v>
+      </c>
+      <c r="W17" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="X17" s="22">
+        <v>0.83773739999999997</v>
+      </c>
+      <c r="AD17" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="6"/>
@@ -1417,7 +1529,7 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="8">
+      <c r="K18" s="32">
         <v>0.83773739999999997</v>
       </c>
       <c r="M18" s="2">
@@ -1433,14 +1545,23 @@
         <v>9</v>
       </c>
       <c r="Q18" s="17">
-        <v>9.0000000000000036</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="X18" s="32">
+        <v>0.83568200000000004</v>
+      </c>
+      <c r="AD18" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="6"/>
@@ -1453,16 +1574,21 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
-      <c r="K19" s="8">
+      <c r="K19" s="32">
         <v>0.83568200000000004</v>
       </c>
-      <c r="X19" s="17"/>
-    </row>
-    <row r="20" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
+      <c r="W19" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="X19" s="22">
+        <v>0.83716539999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="6"/>
@@ -1475,15 +1601,24 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
-      <c r="K20" s="8">
+      <c r="K20" s="32">
         <v>0.83716539999999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="W20" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="X20" s="32">
+        <v>0.83637340000000004</v>
+      </c>
+      <c r="AA20" s="33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="6"/>
@@ -1496,15 +1631,30 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
-      <c r="K21" s="8">
+      <c r="K21" s="32">
         <v>0.83637340000000004</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+      <c r="W21" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="X21" s="22">
+        <v>0.83815379999999995</v>
+      </c>
+      <c r="Z21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA21" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB21" s="22">
+        <v>0.83844677000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="6"/>
@@ -1517,13 +1667,30 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+      <c r="K22" s="32">
+        <v>0.83815379999999995</v>
+      </c>
+      <c r="W22" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="X22" s="22">
+        <v>0.83748688000000004</v>
+      </c>
+      <c r="Z22" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA22" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB22" s="22">
+        <v>0.83815379999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="6"/>
@@ -1536,16 +1703,30 @@
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="AC23" s="2">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="30" t="s">
+      <c r="K23" s="32">
+        <v>0.83748688000000004</v>
+      </c>
+      <c r="W23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="X23" s="22">
+        <v>0.83844677000000001</v>
+      </c>
+      <c r="Z23" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA23" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB23" s="22">
+        <v>0.83795830000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="6"/>
@@ -1558,13 +1739,30 @@
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-    </row>
-    <row r="25" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
+      <c r="K24" s="32">
+        <v>0.83844677000000001</v>
+      </c>
+      <c r="W24" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="X24" s="32">
+        <v>0.83622465999999995</v>
+      </c>
+      <c r="Z24" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA24" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB24" s="22">
+        <v>0.83773739999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="6"/>
@@ -1577,13 +1775,30 @@
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-    </row>
-    <row r="26" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="30" t="s">
+      <c r="K25" s="32">
+        <v>0.83622465999999995</v>
+      </c>
+      <c r="W25" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="X25" s="32">
+        <v>0.83633111000000004</v>
+      </c>
+      <c r="Z25" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA25" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB25" s="22">
+        <v>0.83748688000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="6"/>
@@ -1596,13 +1811,21 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
+      <c r="K26" s="32">
+        <v>0.83633111000000004</v>
+      </c>
+      <c r="W26" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="X26" s="32">
+        <v>0.83674999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="6"/>
@@ -1615,35 +1838,37 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="K27" s="32">
+        <v>0.83674999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="25" t="s">
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-    </row>
-    <row r="30" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="23"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+    </row>
+    <row r="30" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="28"/>
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
@@ -1669,7 +1894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>54</v>
       </c>
@@ -1686,7 +1911,7 @@
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>55</v>
       </c>
@@ -1768,32 +1993,32 @@
       <c r="K36" s="8"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="25" t="s">
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
     </row>
     <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="23"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="28"/>
       <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
@@ -1920,32 +2145,32 @@
       <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D45" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="25" t="s">
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
     </row>
     <row r="46" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="23"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="28"/>
       <c r="D46" s="3" t="s">
         <v>5</v>
       </c>
@@ -2065,32 +2290,32 @@
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="24" t="s">
+      <c r="D53" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="25" t="s">
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="30"/>
+      <c r="K53" s="30"/>
     </row>
     <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="23"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="28"/>
       <c r="D54" s="3" t="s">
         <v>5</v>
       </c>
@@ -2210,32 +2435,32 @@
       <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="24" t="s">
+      <c r="D61" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="25" t="s">
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I61" s="25"/>
-      <c r="J61" s="25"/>
-      <c r="K61" s="25"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="30"/>
     </row>
     <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="21"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="23"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="28"/>
       <c r="D62" s="3" t="s">
         <v>5</v>
       </c>
@@ -2355,32 +2580,32 @@
       <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="C69" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D69" s="24" t="s">
+      <c r="D69" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="25" t="s">
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I69" s="25"/>
-      <c r="J69" s="25"/>
-      <c r="K69" s="25"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
     </row>
     <row r="70" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="21"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="23"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="28"/>
       <c r="D70" s="3" t="s">
         <v>5</v>
       </c>
@@ -2500,32 +2725,32 @@
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="22" t="s">
+      <c r="C77" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="24" t="s">
+      <c r="D77" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="25" t="s">
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I77" s="25"/>
-      <c r="J77" s="25"/>
-      <c r="K77" s="25"/>
+      <c r="I77" s="30"/>
+      <c r="J77" s="30"/>
+      <c r="K77" s="30"/>
     </row>
     <row r="78" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="21"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="23"/>
+      <c r="A78" s="26"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="28"/>
       <c r="D78" s="3" t="s">
         <v>5</v>
       </c>
@@ -2645,32 +2870,32 @@
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="22" t="s">
+      <c r="C85" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="24" t="s">
+      <c r="D85" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="25" t="s">
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I85" s="25"/>
-      <c r="J85" s="25"/>
-      <c r="K85" s="25"/>
+      <c r="I85" s="30"/>
+      <c r="J85" s="30"/>
+      <c r="K85" s="30"/>
     </row>
     <row r="86" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="21"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="23"/>
+      <c r="A86" s="26"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="28"/>
       <c r="D86" s="3" t="s">
         <v>5</v>
       </c>
@@ -2790,32 +3015,32 @@
       <c r="G92" s="7"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" s="20" t="s">
+      <c r="A93" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="B93" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C93" s="22" t="s">
+      <c r="C93" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D93" s="24" t="s">
+      <c r="D93" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
-      <c r="H93" s="25" t="s">
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I93" s="25"/>
-      <c r="J93" s="25"/>
-      <c r="K93" s="25"/>
+      <c r="I93" s="30"/>
+      <c r="J93" s="30"/>
+      <c r="K93" s="30"/>
     </row>
     <row r="94" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="21"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="23"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="28"/>
       <c r="D94" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>